<commit_message>
Added 10k pulldown on SCR
</commit_message>
<xml_diff>
--- a/V4.0 In Development/List of Parts (V4.0).xlsx
+++ b/V4.0 In Development/List of Parts (V4.0).xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koltin Kosik-Harvey\Documents\GitHub\Auxillary-Power-Board\V4.0 In Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koltin.KoltinPC\Documents\GitHub\Auxillary-Power-Board\V4.0 In Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="240">
   <si>
     <t>Part Name</t>
   </si>
@@ -492,9 +492,6 @@
     <t>https://www.digikey.ca/products/en/resistors/through-hole-resistors/53?k=Resistor&amp;k=&amp;pkeyword=Resistor&amp;pv1=475&amp;FV=1c00c5%2C1c0002%2C1f140000%2Cffe00035%2C80009&amp;mnonly=0&amp;newproducts=0&amp;ColumnSort=0&amp;page=1&amp;quantity=0&amp;ptm=0&amp;fid=0&amp;pageSize=25</t>
   </si>
   <si>
-    <t>Biasing the Zener diodes</t>
-  </si>
-  <si>
     <t>Resistor 100 0805</t>
   </si>
   <si>
@@ -742,6 +739,15 @@
   </si>
   <si>
     <t>For the -12V Charge Pump</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Voltage divider bias for op amp </t>
+  </si>
+  <si>
+    <t>Op-Amp Gain / Feedback for 12V reg. / pulldown for crowbar</t>
+  </si>
+  <si>
+    <t>Biasing the Zener diodes (high wattage for safety)</t>
   </si>
 </sst>
 </file>
@@ -1312,24 +1318,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.08984375"/>
-    <col min="2" max="2" width="34.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.6328125"/>
-    <col min="4" max="4" width="13.1796875" style="2"/>
-    <col min="5" max="5" width="13.1796875" style="3"/>
-    <col min="6" max="6" width="65.26953125"/>
-    <col min="7" max="7" width="8.54296875"/>
-    <col min="8" max="8" width="24.26953125"/>
-    <col min="9" max="1025" width="8.54296875"/>
+    <col min="1" max="1" width="32.140625"/>
+    <col min="2" max="2" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5703125"/>
+    <col min="4" max="4" width="13.140625" style="2"/>
+    <col min="5" max="5" width="13.140625" style="3"/>
+    <col min="6" max="6" width="65.28515625"/>
+    <col min="7" max="7" width="8.5703125"/>
+    <col min="8" max="8" width="24.28515625"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1349,7 +1355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1369,7 +1375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1389,7 +1395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1409,7 +1415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1429,7 +1435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1449,7 +1455,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1469,7 +1475,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1489,7 +1495,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1509,7 +1515,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1529,7 +1535,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1549,7 +1555,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1569,7 +1575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1589,7 +1595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1609,7 +1615,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1629,7 +1635,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1649,7 +1655,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1669,7 +1675,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1689,7 +1695,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1709,7 +1715,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -1729,7 +1735,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1749,7 +1755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1769,7 +1775,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1789,7 +1795,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1809,7 +1815,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1829,7 +1835,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -1849,7 +1855,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -1869,7 +1875,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -1889,7 +1895,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -1909,15 +1915,15 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>233</v>
+      </c>
+      <c r="B30" s="23" t="s">
         <v>234</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="C30" s="12" t="s">
         <v>235</v>
-      </c>
-      <c r="C30" s="12" t="s">
-        <v>236</v>
       </c>
       <c r="D30" s="2">
         <v>0.27</v>
@@ -1926,10 +1932,10 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -1946,7 +1952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -1963,7 +1969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -1980,7 +1986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -2000,7 +2006,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -2017,7 +2023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -2034,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>130</v>
       </c>
@@ -2051,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -2065,13 +2071,13 @@
         <v>0.15</v>
       </c>
       <c r="E38" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F38" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -2085,13 +2091,13 @@
         <v>0.15</v>
       </c>
       <c r="E39" s="13">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>140</v>
       </c>
@@ -2111,7 +2117,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>144</v>
       </c>
@@ -2131,7 +2137,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>148</v>
       </c>
@@ -2148,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>151</v>
       </c>
@@ -2165,18 +2171,18 @@
         <v>2</v>
       </c>
       <c r="F43" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="B44" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>156</v>
-      </c>
-      <c r="C44" s="9" t="s">
-        <v>157</v>
       </c>
       <c r="D44" s="2">
         <v>0.15</v>
@@ -2185,31 +2191,31 @@
         <v>1</v>
       </c>
       <c r="F44" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="19"/>
       <c r="C45" s="9"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B46" s="19"/>
       <c r="C46" s="9"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C47" s="9"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B48" s="20"/>
       <c r="C48" s="9"/>
     </row>
-    <row r="49" spans="1:2" ht="40" x14ac:dyDescent="1.1000000000000001">
+    <row r="49" spans="1:2" ht="40.5" x14ac:dyDescent="0.75">
       <c r="A49" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B49" s="22">
         <f>SUMPRODUCT(D2:D66, E2:E66)</f>
-        <v>88.149000000000029</v>
+        <v>88.149000000000044</v>
       </c>
     </row>
   </sheetData>
@@ -2247,20 +2253,20 @@
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.08984375"/>
-    <col min="2" max="2" width="30.7265625" style="1"/>
-    <col min="3" max="3" width="22.6328125"/>
-    <col min="4" max="4" width="13.1796875" style="2"/>
-    <col min="5" max="5" width="13.1796875" style="3"/>
-    <col min="6" max="6" width="65.26953125"/>
-    <col min="7" max="7" width="8.54296875"/>
-    <col min="8" max="8" width="24.26953125"/>
-    <col min="9" max="1025" width="8.54296875"/>
+    <col min="1" max="1" width="32.140625"/>
+    <col min="2" max="2" width="30.7109375" style="1"/>
+    <col min="3" max="3" width="22.5703125"/>
+    <col min="4" max="4" width="13.140625" style="2"/>
+    <col min="5" max="5" width="13.140625" style="3"/>
+    <col min="6" max="6" width="65.28515625"/>
+    <col min="7" max="7" width="8.5703125"/>
+    <col min="8" max="8" width="24.28515625"/>
+    <col min="9" max="1025" width="8.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2280,15 +2286,15 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>160</v>
-      </c>
-      <c r="C2" s="9" t="s">
-        <v>161</v>
       </c>
       <c r="D2" s="2">
         <v>3.58</v>
@@ -2297,18 +2303,18 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>163</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="D3" s="2">
         <v>6.22</v>
@@ -2317,18 +2323,18 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="9" t="s">
         <v>166</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>167</v>
       </c>
       <c r="D4" s="2">
         <v>3.3</v>
@@ -2340,15 +2346,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="17" t="s">
         <v>168</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="C5" s="9" t="s">
         <v>169</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="D5" s="2">
         <v>0.47</v>
@@ -2357,18 +2363,18 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C6" s="9" t="s">
         <v>172</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>173</v>
       </c>
       <c r="D6" s="2">
         <v>2.61</v>
@@ -2377,18 +2383,18 @@
         <v>1</v>
       </c>
       <c r="F6" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>175</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>176</v>
       </c>
       <c r="D7" s="2">
         <v>3.56</v>
@@ -2400,7 +2406,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2420,7 +2426,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2440,7 +2446,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2460,15 +2466,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>176</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="9" t="s">
         <v>178</v>
-      </c>
-      <c r="C11" s="9" t="s">
-        <v>179</v>
       </c>
       <c r="D11" s="2">
         <v>2.57</v>
@@ -2477,18 +2483,18 @@
         <v>2</v>
       </c>
       <c r="F11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="B12" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="9" t="s">
         <v>182</v>
-      </c>
-      <c r="C12" s="9" t="s">
-        <v>183</v>
       </c>
       <c r="D12" s="2">
         <v>0.67</v>
@@ -2497,10 +2503,10 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2520,15 +2526,15 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B14" s="1">
         <v>3568</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D14" s="2">
         <v>1.66</v>
@@ -2537,18 +2543,18 @@
         <v>1</v>
       </c>
       <c r="F14" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>187</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B15" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="9" t="s">
         <v>189</v>
-      </c>
-      <c r="C15" s="9" t="s">
-        <v>190</v>
       </c>
       <c r="D15" s="2">
         <v>1.55</v>
@@ -2557,18 +2563,18 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="B16" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="9" t="s">
         <v>193</v>
-      </c>
-      <c r="C16" s="9" t="s">
-        <v>194</v>
       </c>
       <c r="D16" s="2">
         <v>5.03</v>
@@ -2577,10 +2583,10 @@
         <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -2600,7 +2606,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -2620,9 +2626,9 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>115</v>
@@ -2637,9 +2643,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>118</v>
@@ -2654,9 +2660,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B21" s="17" t="s">
         <v>121</v>
@@ -2671,18 +2677,18 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="B22" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="B22" s="17" t="s">
+      <c r="C22" s="9" t="s">
         <v>201</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>202</v>
       </c>
       <c r="D22" s="2">
         <v>1.1599999999999999</v>
@@ -2691,18 +2697,18 @@
         <v>1</v>
       </c>
       <c r="F22" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
+      <c r="B23" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="B23" s="1" t="s">
+      <c r="C23" s="9" t="s">
         <v>205</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>206</v>
       </c>
       <c r="D23" s="2">
         <v>1.44</v>
@@ -2714,15 +2720,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>206</v>
+      </c>
+      <c r="B24" s="17" t="s">
         <v>207</v>
       </c>
-      <c r="B24" s="17" t="s">
+      <c r="C24" s="9" t="s">
         <v>208</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>209</v>
       </c>
       <c r="D24" s="2">
         <v>1.1599999999999999</v>
@@ -2734,7 +2740,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -2754,15 +2760,15 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>209</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="B26" s="1" t="s">
+      <c r="C26" s="9" t="s">
         <v>211</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>212</v>
       </c>
       <c r="D26" s="2">
         <v>4.2699999999999996</v>
@@ -2771,18 +2777,18 @@
         <v>1</v>
       </c>
       <c r="F26" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+      <c r="B27" s="20" t="s">
         <v>214</v>
       </c>
-      <c r="B27" s="20" t="s">
+      <c r="C27" s="9" t="s">
         <v>215</v>
-      </c>
-      <c r="C27" s="9" t="s">
-        <v>216</v>
       </c>
       <c r="D27" s="2">
         <v>4.1100000000000003</v>
@@ -2791,18 +2797,18 @@
         <v>1</v>
       </c>
       <c r="F27" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>213</v>
+      </c>
+      <c r="B28" s="20" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>214</v>
-      </c>
-      <c r="B28" s="20" t="s">
+      <c r="C28" s="9" t="s">
         <v>218</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>219</v>
       </c>
       <c r="D28" s="2">
         <v>1.03</v>
@@ -2811,18 +2817,18 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>220</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>221</v>
       </c>
       <c r="B29" s="19">
         <v>9900</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D29" s="2">
         <v>0.14000000000000001</v>
@@ -2831,18 +2837,18 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>224</v>
       </c>
       <c r="B30" s="19">
         <v>4694</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D30" s="2">
         <v>0.14000000000000001</v>
@@ -2851,18 +2857,18 @@
         <v>2</v>
       </c>
       <c r="F30" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B31" s="1">
         <v>4672</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D31" s="2">
         <v>0.22</v>
@@ -2871,18 +2877,18 @@
         <v>0</v>
       </c>
       <c r="F31" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+      <c r="B32" s="20" t="s">
         <v>229</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="C32" s="9" t="s">
         <v>230</v>
-      </c>
-      <c r="C32" s="9" t="s">
-        <v>231</v>
       </c>
       <c r="D32" s="2">
         <v>0.26</v>
@@ -2891,26 +2897,26 @@
         <v>0</v>
       </c>
       <c r="F32" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" ht="40" x14ac:dyDescent="1.1000000000000001">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" ht="40.5" x14ac:dyDescent="0.75">
       <c r="A33" s="21" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B33" s="22">
         <f>SUMPRODUCT(D2:D50, E2:E50)</f>
         <v>72.789999999999992</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>232</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>233</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made some updates, generated BRD file
-Used a 10k bridging resistor at battery input
-forgot to fully connected the SCR to the negative terminal (fixed it)
-Generated board file. Maximum demention for board is 10cmX10cm. May
have to utlize the other side of the board to make it smaller.
</commit_message>
<xml_diff>
--- a/V4.0 In Development/List of Parts (V4.0).xlsx
+++ b/V4.0 In Development/List of Parts (V4.0).xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18067"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18229"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koltin.KoltinPC\Documents\GitHub\Auxillary-Power-Board\V4.0 In Development\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Koltin Kosik-Harvey\Documents\GitHub\Auxillary-Power-Board\V4.0 In Development\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="V3.4" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">V4.0!$A$1:$F$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'V4.0'!$A$1:$F$44</definedName>
   </definedNames>
   <calcPr calcId="171027" iterateDelta="1E-4"/>
   <extLst>
@@ -1318,24 +1318,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.140625"/>
-    <col min="2" max="2" width="34.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.5703125"/>
-    <col min="4" max="4" width="13.140625" style="2"/>
-    <col min="5" max="5" width="13.140625" style="3"/>
-    <col min="6" max="6" width="65.28515625"/>
-    <col min="7" max="7" width="8.5703125"/>
-    <col min="8" max="8" width="24.28515625"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="32.1796875"/>
+    <col min="2" max="2" width="34.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.54296875"/>
+    <col min="4" max="4" width="13.1796875" style="2"/>
+    <col min="5" max="5" width="13.1796875" style="3"/>
+    <col min="6" max="6" width="65.26953125"/>
+    <col min="7" max="7" width="8.54296875"/>
+    <col min="8" max="8" width="24.26953125"/>
+    <col min="9" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1355,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -1375,7 +1375,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -1415,7 +1415,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1455,7 +1455,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1475,7 +1475,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>29</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>37</v>
       </c>
@@ -1535,7 +1535,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>41</v>
       </c>
@@ -1555,7 +1555,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>45</v>
       </c>
@@ -1575,7 +1575,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>52</v>
       </c>
@@ -1615,7 +1615,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>56</v>
       </c>
@@ -1635,7 +1635,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>60</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>64</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>68</v>
       </c>
@@ -1695,7 +1695,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>71</v>
       </c>
@@ -1715,7 +1715,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>75</v>
       </c>
@@ -1735,7 +1735,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>79</v>
       </c>
@@ -1755,7 +1755,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>79</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>85</v>
       </c>
@@ -1795,7 +1795,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>88</v>
       </c>
@@ -1815,7 +1815,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>91</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>95</v>
       </c>
@@ -1855,7 +1855,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>99</v>
       </c>
@@ -1875,7 +1875,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>103</v>
       </c>
@@ -1895,7 +1895,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>107</v>
       </c>
@@ -1915,7 +1915,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>233</v>
       </c>
@@ -1935,7 +1935,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>111</v>
       </c>
@@ -1952,7 +1952,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>114</v>
       </c>
@@ -1969,7 +1969,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>117</v>
       </c>
@@ -1986,7 +1986,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>120</v>
       </c>
@@ -2000,13 +2000,13 @@
         <v>0.16</v>
       </c>
       <c r="E34" s="13">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F34" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>124</v>
       </c>
@@ -2023,7 +2023,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>127</v>
       </c>
@@ -2040,7 +2040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>130</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>133</v>
       </c>
@@ -2077,7 +2077,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>137</v>
       </c>
@@ -2091,13 +2091,13 @@
         <v>0.15</v>
       </c>
       <c r="E39" s="13">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F39" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>140</v>
       </c>
@@ -2117,7 +2117,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>144</v>
       </c>
@@ -2137,7 +2137,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>148</v>
       </c>
@@ -2154,7 +2154,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>151</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>154</v>
       </c>
@@ -2194,28 +2194,28 @@
         <v>157</v>
       </c>
     </row>
-    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B45" s="19"/>
       <c r="C45" s="9"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B46" s="19"/>
       <c r="C46" s="9"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C47" s="9"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B48" s="20"/>
       <c r="C48" s="9"/>
     </row>
-    <row r="49" spans="1:2" ht="40.5" x14ac:dyDescent="0.75">
+    <row r="49" spans="1:2" ht="40" x14ac:dyDescent="1.1000000000000001">
       <c r="A49" s="21" t="s">
         <v>158</v>
       </c>
       <c r="B49" s="22">
         <f>SUMPRODUCT(D2:D66, E2:E66)</f>
-        <v>88.149000000000044</v>
+        <v>88.139000000000024</v>
       </c>
     </row>
   </sheetData>
@@ -2253,20 +2253,20 @@
   <sheetViews>
     <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.140625"/>
-    <col min="2" max="2" width="30.7109375" style="1"/>
-    <col min="3" max="3" width="22.5703125"/>
-    <col min="4" max="4" width="13.140625" style="2"/>
-    <col min="5" max="5" width="13.140625" style="3"/>
-    <col min="6" max="6" width="65.28515625"/>
-    <col min="7" max="7" width="8.5703125"/>
-    <col min="8" max="8" width="24.28515625"/>
-    <col min="9" max="1025" width="8.5703125"/>
+    <col min="1" max="1" width="32.1796875"/>
+    <col min="2" max="2" width="30.7265625" style="1"/>
+    <col min="3" max="3" width="22.54296875"/>
+    <col min="4" max="4" width="13.1796875" style="2"/>
+    <col min="5" max="5" width="13.1796875" style="3"/>
+    <col min="6" max="6" width="65.26953125"/>
+    <col min="7" max="7" width="8.54296875"/>
+    <col min="8" max="8" width="24.26953125"/>
+    <col min="9" max="1025" width="8.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -2286,7 +2286,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2326,7 +2326,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -2346,7 +2346,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>167</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>33</v>
       </c>
@@ -2386,7 +2386,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -2406,7 +2406,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>37</v>
       </c>
@@ -2426,7 +2426,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>45</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>49</v>
       </c>
@@ -2466,7 +2466,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>176</v>
       </c>
@@ -2486,7 +2486,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>180</v>
       </c>
@@ -2506,7 +2506,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>68</v>
       </c>
@@ -2526,7 +2526,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>184</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>187</v>
       </c>
@@ -2566,7 +2566,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>191</v>
       </c>
@@ -2586,7 +2586,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>79</v>
       </c>
@@ -2606,7 +2606,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>107</v>
       </c>
@@ -2626,7 +2626,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>195</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>196</v>
       </c>
@@ -2660,7 +2660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>197</v>
       </c>
@@ -2680,7 +2680,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>199</v>
       </c>
@@ -2700,7 +2700,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>203</v>
       </c>
@@ -2720,7 +2720,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>206</v>
       </c>
@@ -2740,7 +2740,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>140</v>
       </c>
@@ -2760,7 +2760,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>209</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>213</v>
       </c>
@@ -2800,7 +2800,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>213</v>
       </c>
@@ -2820,7 +2820,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="16.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>220</v>
       </c>
@@ -2840,7 +2840,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>223</v>
       </c>
@@ -2860,7 +2860,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>225</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>228</v>
       </c>
@@ -2900,7 +2900,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="40.5" x14ac:dyDescent="0.75">
+    <row r="33" spans="1:2" ht="40" x14ac:dyDescent="1.1000000000000001">
       <c r="A33" s="21" t="s">
         <v>158</v>
       </c>
@@ -2909,12 +2909,12 @@
         <v>72.789999999999992</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>231</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>232</v>
       </c>

</xml_diff>